<commit_message>
fixing payments aligning, fix specific fixes add canceling analysis
</commit_message>
<xml_diff>
--- a/data/handling duplicates.xlsx
+++ b/data/handling duplicates.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="89">
   <si>
     <t>Customer Email</t>
   </si>
@@ -297,20 +297,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="177"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -321,18 +314,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -347,11 +334,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -635,14 +620,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D91"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="31.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -692,7 +678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" s="2" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -701,6 +687,9 @@
       </c>
       <c r="C5" s="2">
         <v>1</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
@@ -714,28 +703,28 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="7" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="2">
         <v>2</v>
       </c>
-      <c r="D7" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="D7" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="2">
         <v>2</v>
       </c>
     </row>
@@ -749,6 +738,9 @@
       <c r="C9" s="2">
         <v>3</v>
       </c>
+      <c r="D9" s="2" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="10" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
@@ -926,8 +918,8 @@
       <c r="C24">
         <v>21</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>87</v>
+      <c r="D24" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
@@ -1327,53 +1319,53 @@
         <v>140</v>
       </c>
     </row>
-    <row r="57" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="3" t="s">
+    <row r="57" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="B57" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C57" s="3">
+      <c r="C57" s="1">
         <v>141</v>
       </c>
-      <c r="D57" s="3" t="s">
+      <c r="D57" s="1" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="58" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="3" t="s">
+    <row r="58" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B58" s="3" t="s">
+      <c r="B58" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C58" s="3">
+      <c r="C58" s="1">
         <v>141</v>
       </c>
     </row>
-    <row r="59" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="4" t="s">
+    <row r="59" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B59" s="4" t="s">
+      <c r="B59" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C59" s="4">
+      <c r="C59" s="2">
         <v>148</v>
       </c>
-      <c r="D59" s="4" t="s">
+      <c r="D59" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="60" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="4" t="s">
+    <row r="60" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B60" s="4" t="s">
+      <c r="B60" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C60" s="4">
+      <c r="C60" s="2">
         <v>148</v>
       </c>
     </row>
@@ -1524,7 +1516,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>70</v>
       </c>
@@ -1535,7 +1527,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" ht="12.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>72</v>
       </c>
@@ -1654,50 +1646,50 @@
         <v>190</v>
       </c>
     </row>
-    <row r="84" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="4" t="s">
+    <row r="84" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B84" s="4" t="s">
+      <c r="B84" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C84" s="4">
+      <c r="C84" s="2">
         <v>205</v>
       </c>
-      <c r="D84" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="4" t="s">
+      <c r="D84" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B85" s="4" t="s">
+      <c r="B85" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C85" s="4">
+      <c r="C85" s="2">
         <v>205</v>
       </c>
     </row>
-    <row r="86" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="4" t="s">
+    <row r="86" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B86" s="4" t="s">
+      <c r="B86" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C86" s="4">
+      <c r="C86" s="2">
         <v>205</v>
       </c>
     </row>
-    <row r="87" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="4" t="s">
+    <row r="87" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B87" s="4" t="s">
+      <c r="B87" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C87" s="4">
+      <c r="C87" s="2">
         <v>205</v>
       </c>
     </row>

</xml_diff>